<commit_message>
Add conclusiones de CC + tiempos de ejecución
</commit_message>
<xml_diff>
--- a/Analisis/GraficoTiempos.xlsx
+++ b/Analisis/GraficoTiempos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mica\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mica\workspace\TallerProgra\fork_mramirez\tpComplejidad\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -176,22 +176,22 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2867,8 +2867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2878,946 +2878,946 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="12"/>
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="11">
+      <c r="A4" s="9">
         <v>400</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="6">
         <v>1</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>1</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>1</v>
       </c>
-      <c r="E4" s="4">
-        <v>0</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="4">
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>600</v>
       </c>
-      <c r="B5" s="8">
-        <v>0</v>
-      </c>
-      <c r="C5" s="6">
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5">
         <v>1</v>
       </c>
-      <c r="D5" s="4">
-        <v>0</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0</v>
-      </c>
-      <c r="G5" s="4">
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>800</v>
       </c>
-      <c r="B6" s="8">
-        <v>0</v>
-      </c>
-      <c r="C6" s="6">
+      <c r="B6" s="6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5">
         <v>2</v>
       </c>
-      <c r="D6" s="4">
-        <v>0</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0</v>
-      </c>
-      <c r="G6" s="4">
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>1000</v>
       </c>
-      <c r="B7" s="8">
-        <v>0</v>
-      </c>
-      <c r="C7" s="6">
+      <c r="B7" s="6">
+        <v>0</v>
+      </c>
+      <c r="C7" s="5">
         <v>2</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>1</v>
       </c>
-      <c r="E7" s="4">
-        <v>0</v>
-      </c>
-      <c r="F7" s="4">
-        <v>0</v>
-      </c>
-      <c r="G7" s="4">
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>1200</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="6">
         <v>1</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>2</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>1</v>
       </c>
-      <c r="E8" s="4">
-        <v>0</v>
-      </c>
-      <c r="F8" s="4">
-        <v>0</v>
-      </c>
-      <c r="G8" s="4">
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>1400</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="6">
         <v>1</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>3</v>
       </c>
-      <c r="D9" s="4">
-        <v>0</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0</v>
-      </c>
-      <c r="F9" s="4">
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
         <v>1</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>1600</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="6">
         <v>2</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>3</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>1</v>
       </c>
-      <c r="E10" s="4">
-        <v>0</v>
-      </c>
-      <c r="F10" s="4">
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
         <v>1</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>1800</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="6">
         <v>2</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>4</v>
       </c>
-      <c r="D11" s="4">
-        <v>0</v>
-      </c>
-      <c r="E11" s="4">
-        <v>0</v>
-      </c>
-      <c r="F11" s="4">
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
         <v>1</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>2000</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="6">
         <v>3</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>5</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>1</v>
       </c>
-      <c r="E12" s="4">
-        <v>0</v>
-      </c>
-      <c r="F12" s="4">
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
         <v>1</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>2200</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="6">
         <v>3</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>7</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>1</v>
       </c>
-      <c r="E13" s="4">
-        <v>0</v>
-      </c>
-      <c r="F13" s="4">
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
         <v>1</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>2400</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="6">
         <v>3</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>8</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
         <v>1</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>1</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="3">
         <v>1</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>2600</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="6">
         <v>4</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>9</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <v>1</v>
       </c>
-      <c r="E15" s="4">
-        <v>0</v>
-      </c>
-      <c r="F15" s="4">
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
         <v>1</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>2800</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="6">
         <v>4</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="5">
         <v>11</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
         <v>2</v>
       </c>
-      <c r="E16" s="4">
-        <v>0</v>
-      </c>
-      <c r="F16" s="4">
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
         <v>1</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="A17" s="3">
         <v>3000</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="6">
         <v>6</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <v>14</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <v>2</v>
       </c>
-      <c r="E17" s="4">
-        <v>0</v>
-      </c>
-      <c r="F17" s="4">
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
         <v>1</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>3200</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="6">
         <v>6</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="5">
         <v>15</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="3">
         <v>1</v>
       </c>
-      <c r="E18" s="4">
-        <v>0</v>
-      </c>
-      <c r="F18" s="4">
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
         <v>1</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>3400</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="6">
         <v>7</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="5">
         <v>16</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="3">
         <v>2</v>
       </c>
-      <c r="E19" s="4">
-        <v>0</v>
-      </c>
-      <c r="F19" s="4">
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
         <v>1</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>3600</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="6">
         <v>7</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="5">
         <v>19</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="3">
         <v>2</v>
       </c>
-      <c r="E20" s="4">
-        <v>0</v>
-      </c>
-      <c r="F20" s="4">
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
         <v>2</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+      <c r="A21" s="3">
         <v>3800</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="6">
         <v>9</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="5">
         <v>20</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="3">
         <v>2</v>
       </c>
-      <c r="E21" s="4">
-        <v>0</v>
-      </c>
-      <c r="F21" s="4">
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
         <v>2</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>4000</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22" s="6">
         <v>10</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="5">
         <v>23</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="3">
         <v>2</v>
       </c>
-      <c r="E22" s="4">
-        <v>0</v>
-      </c>
-      <c r="F22" s="4">
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
         <v>2</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G22" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+      <c r="A23" s="3">
         <v>4200</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23" s="6">
         <v>10</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="5">
         <v>25</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="3">
         <v>2</v>
       </c>
-      <c r="E23" s="4">
-        <v>0</v>
-      </c>
-      <c r="F23" s="4">
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3">
         <v>2</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G23" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
+      <c r="A24" s="3">
         <v>4400</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24" s="7">
         <v>11</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C24" s="3">
         <v>27</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="3">
         <v>3</v>
       </c>
-      <c r="E24" s="4">
-        <v>0</v>
-      </c>
-      <c r="F24" s="4">
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
         <v>1</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+      <c r="A25" s="3">
         <v>4600</v>
       </c>
-      <c r="B25" s="9">
+      <c r="B25" s="7">
         <v>13</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="3">
         <v>31</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="3">
         <v>2</v>
       </c>
-      <c r="E25" s="4">
-        <v>0</v>
-      </c>
-      <c r="F25" s="4">
+      <c r="E25" s="3">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3">
         <v>2</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+      <c r="A26" s="3">
         <v>4800</v>
       </c>
-      <c r="B26" s="9">
+      <c r="B26" s="7">
         <v>14</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="3">
         <v>33</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D26" s="3">
         <v>3</v>
       </c>
-      <c r="E26" s="4">
-        <v>0</v>
-      </c>
-      <c r="F26" s="4">
+      <c r="E26" s="3">
+        <v>0</v>
+      </c>
+      <c r="F26" s="3">
         <v>2</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G26" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+      <c r="A27" s="3">
         <v>5000</v>
       </c>
-      <c r="B27" s="9">
+      <c r="B27" s="7">
         <v>14</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="3">
         <v>37</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D27" s="3">
         <v>3</v>
       </c>
-      <c r="E27" s="4">
-        <v>0</v>
-      </c>
-      <c r="F27" s="4">
+      <c r="E27" s="3">
+        <v>0</v>
+      </c>
+      <c r="F27" s="3">
         <v>2</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G27" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+      <c r="A28" s="3">
         <v>5200</v>
       </c>
-      <c r="B28" s="9">
+      <c r="B28" s="7">
         <v>16</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="3">
         <v>39</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="3">
         <v>2</v>
       </c>
-      <c r="E28" s="4">
-        <v>0</v>
-      </c>
-      <c r="F28" s="4">
+      <c r="E28" s="3">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3">
         <v>2</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+      <c r="A29" s="3">
         <v>5400</v>
       </c>
-      <c r="B29" s="9">
+      <c r="B29" s="7">
         <v>17</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="3">
         <v>42</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="3">
         <v>3</v>
       </c>
-      <c r="E29" s="4">
-        <v>0</v>
-      </c>
-      <c r="F29" s="4">
+      <c r="E29" s="3">
+        <v>0</v>
+      </c>
+      <c r="F29" s="3">
         <v>2</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+      <c r="A30" s="3">
         <v>5600</v>
       </c>
-      <c r="B30" s="9">
+      <c r="B30" s="7">
         <v>18</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="3">
         <v>44</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="3">
         <v>3</v>
       </c>
-      <c r="E30" s="4">
-        <v>0</v>
-      </c>
-      <c r="F30" s="4">
+      <c r="E30" s="3">
+        <v>0</v>
+      </c>
+      <c r="F30" s="3">
         <v>2</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
+      <c r="A31" s="3">
         <v>5800</v>
       </c>
-      <c r="B31" s="9">
+      <c r="B31" s="7">
         <v>20</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="3">
         <v>49</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D31" s="3">
         <v>3</v>
       </c>
-      <c r="E31" s="4">
-        <v>0</v>
-      </c>
-      <c r="F31" s="4">
+      <c r="E31" s="3">
+        <v>0</v>
+      </c>
+      <c r="F31" s="3">
         <v>2</v>
       </c>
-      <c r="G31" s="4">
+      <c r="G31" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+      <c r="A32" s="3">
         <v>6000</v>
       </c>
-      <c r="B32" s="9">
+      <c r="B32" s="7">
         <v>22</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="3">
         <v>52</v>
       </c>
-      <c r="D32" s="4">
+      <c r="D32" s="3">
         <v>2</v>
       </c>
-      <c r="E32" s="4">
-        <v>0</v>
-      </c>
-      <c r="F32" s="4">
+      <c r="E32" s="3">
+        <v>0</v>
+      </c>
+      <c r="F32" s="3">
         <v>3</v>
       </c>
-      <c r="G32" s="4">
+      <c r="G32" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
+      <c r="A33" s="3">
         <v>6200</v>
       </c>
-      <c r="B33" s="9">
+      <c r="B33" s="7">
         <v>23</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="3">
         <v>55</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D33" s="3">
         <v>3</v>
       </c>
-      <c r="E33" s="4">
-        <v>0</v>
-      </c>
-      <c r="F33" s="4">
+      <c r="E33" s="3">
+        <v>0</v>
+      </c>
+      <c r="F33" s="3">
         <v>2</v>
       </c>
-      <c r="G33" s="4">
+      <c r="G33" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
+      <c r="A34" s="3">
         <v>6400</v>
       </c>
-      <c r="B34" s="9">
+      <c r="B34" s="7">
         <v>25</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="3">
         <v>59</v>
       </c>
-      <c r="D34" s="4">
+      <c r="D34" s="3">
         <v>3</v>
       </c>
-      <c r="E34" s="4">
-        <v>0</v>
-      </c>
-      <c r="F34" s="4">
+      <c r="E34" s="3">
+        <v>0</v>
+      </c>
+      <c r="F34" s="3">
         <v>3</v>
       </c>
-      <c r="G34" s="4">
+      <c r="G34" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
+      <c r="A35" s="3">
         <v>6600</v>
       </c>
-      <c r="B35" s="9">
+      <c r="B35" s="7">
         <v>26</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35" s="3">
         <v>62</v>
       </c>
-      <c r="D35" s="4">
+      <c r="D35" s="3">
         <v>4</v>
       </c>
-      <c r="E35" s="4">
-        <v>0</v>
-      </c>
-      <c r="F35" s="4">
+      <c r="E35" s="3">
+        <v>0</v>
+      </c>
+      <c r="F35" s="3">
         <v>3</v>
       </c>
-      <c r="G35" s="4">
+      <c r="G35" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
+      <c r="A36" s="3">
         <v>6800</v>
       </c>
-      <c r="B36" s="9">
+      <c r="B36" s="7">
         <v>27</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36" s="3">
         <v>67</v>
       </c>
-      <c r="D36" s="4">
+      <c r="D36" s="3">
         <v>3</v>
       </c>
-      <c r="E36" s="4">
-        <v>0</v>
-      </c>
-      <c r="F36" s="4">
+      <c r="E36" s="3">
+        <v>0</v>
+      </c>
+      <c r="F36" s="3">
         <v>3</v>
       </c>
-      <c r="G36" s="4">
+      <c r="G36" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="5">
+      <c r="A37" s="4">
         <v>7000</v>
       </c>
-      <c r="B37" s="10">
+      <c r="B37" s="8">
         <v>29</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C37" s="4">
         <v>71</v>
       </c>
-      <c r="D37" s="5">
+      <c r="D37" s="4">
         <v>3</v>
       </c>
-      <c r="E37" s="5">
-        <v>0</v>
-      </c>
-      <c r="F37" s="5">
+      <c r="E37" s="4">
+        <v>0</v>
+      </c>
+      <c r="F37" s="4">
         <v>3</v>
       </c>
-      <c r="G37" s="5">
+      <c r="G37" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
+      <c r="A44" s="10"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
+      <c r="A45" s="10"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
-      <c r="B46" s="12"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
+      <c r="A46" s="10"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="12"/>
-      <c r="B47" s="12"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
+      <c r="A47" s="10"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="12"/>
-      <c r="B48" s="12"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="12"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
+      <c r="A48" s="10"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="12"/>
-      <c r="B49" s="12"/>
-      <c r="C49" s="12"/>
-      <c r="D49" s="12"/>
-      <c r="E49" s="12"/>
-      <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
+      <c r="A49" s="10"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="12"/>
-      <c r="B50" s="12"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
-      <c r="G50" s="12"/>
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="12"/>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
+      <c r="A51" s="10"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Add Gráfico tiempos BinomioDeNewton + coefUsandoMat
</commit_message>
<xml_diff>
--- a/Analisis/GraficoTiempos.xlsx
+++ b/Analisis/GraficoTiempos.xlsx
@@ -5,14 +5,15 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mica\workspace\TallerProgra\fork_mramirez\tpComplejidad\Analisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2017_1C\PrograAvanzada\tpComplejidad\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Datos + Gráfico" sheetId="1" r:id="rId1"/>
+    <sheet name="Polinomio" sheetId="1" r:id="rId1"/>
+    <sheet name="Binomio de Newton" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Recursiva</t>
   </si>
@@ -48,6 +49,24 @@
   </si>
   <si>
     <t>Tiempo en ms</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>Num combinatorio según</t>
+  </si>
+  <si>
+    <t>Recursividad</t>
+  </si>
+  <si>
+    <t>Sin recursividad</t>
+  </si>
+  <si>
+    <t>Usando matriz</t>
   </si>
 </sst>
 </file>
@@ -174,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -192,6 +211,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -290,7 +316,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Datos + Gráfico'!$B$3</c:f>
+              <c:f>Polinomio!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -313,7 +339,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Datos + Gráfico'!$A$4:$A$37</c:f>
+              <c:f>Polinomio!$A$4:$A$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
@@ -424,7 +450,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Datos + Gráfico'!$B$4:$B$37</c:f>
+              <c:f>Polinomio!$B$4:$B$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
@@ -545,7 +571,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Datos + Gráfico'!$C$3</c:f>
+              <c:f>Polinomio!$C$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -568,7 +594,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Datos + Gráfico'!$A$4:$A$37</c:f>
+              <c:f>Polinomio!$A$4:$A$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
@@ -679,7 +705,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Datos + Gráfico'!$C$4:$C$37</c:f>
+              <c:f>Polinomio!$C$4:$C$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
@@ -800,7 +826,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Datos + Gráfico'!$D$3</c:f>
+              <c:f>Polinomio!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -823,7 +849,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Datos + Gráfico'!$A$4:$A$37</c:f>
+              <c:f>Polinomio!$A$4:$A$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
@@ -934,7 +960,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Datos + Gráfico'!$D$4:$D$37</c:f>
+              <c:f>Polinomio!$D$4:$D$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
@@ -1055,7 +1081,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Datos + Gráfico'!$E$3</c:f>
+              <c:f>Polinomio!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1078,7 +1104,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Datos + Gráfico'!$A$4:$A$37</c:f>
+              <c:f>Polinomio!$A$4:$A$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
@@ -1189,7 +1215,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Datos + Gráfico'!$E$4:$E$37</c:f>
+              <c:f>Polinomio!$E$4:$E$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
@@ -1310,7 +1336,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Datos + Gráfico'!$F$3</c:f>
+              <c:f>Polinomio!$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1333,7 +1359,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Datos + Gráfico'!$A$4:$A$37</c:f>
+              <c:f>Polinomio!$A$4:$A$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
@@ -1444,7 +1470,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Datos + Gráfico'!$F$4:$F$37</c:f>
+              <c:f>Polinomio!$F$4:$F$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
@@ -1565,7 +1591,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Datos + Gráfico'!$G$3</c:f>
+              <c:f>Polinomio!$G$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1588,7 +1614,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Datos + Gráfico'!$A$4:$A$37</c:f>
+              <c:f>Polinomio!$A$4:$A$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
@@ -1699,7 +1725,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Datos + Gráfico'!$G$4:$G$37</c:f>
+              <c:f>Polinomio!$G$4:$G$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
@@ -1812,6 +1838,557 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-9CC4-4265-AA32-41AE1FDEF9E2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="888643023"/>
+        <c:axId val="888646767"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="888643023"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="888646767"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="888646767"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="888643023"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Comparación</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Binomio de Newton'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Recursividad</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Binomio de Newton'!$B$3:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Binomio de Newton'!$C$3:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1142</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-EA47-4D74-A630-7E121B6A27D3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Binomio de Newton'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Sin recursividad</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Binomio de Newton'!$B$3:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Binomio de Newton'!$D$3:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-EA47-4D74-A630-7E121B6A27D3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Binomio de Newton'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Usando matriz</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Binomio de Newton'!$B$3:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Binomio de Newton'!$E$3:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-EA47-4D74-A630-7E121B6A27D3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2051,7 +2628,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2586,6 +3719,43 @@
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="11" name="Gráfico 10"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>509589</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Gráfico 9"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2867,7 +4037,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
@@ -3828,4 +4998,176 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0</v>
+      </c>
+      <c r="D3" s="9">
+        <v>0</v>
+      </c>
+      <c r="E3" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>31</v>
+      </c>
+      <c r="B6" s="3">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>41</v>
+      </c>
+      <c r="B7" s="3">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>51</v>
+      </c>
+      <c r="B8" s="3">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3">
+        <v>48</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>61</v>
+      </c>
+      <c r="B9" s="4">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1142</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
evaluarMejorada + Gráfico tiempos + Planilla métrica completa
</commit_message>
<xml_diff>
--- a/Analisis/GraficoTiempos.xlsx
+++ b/Analisis/GraficoTiempos.xlsx
@@ -5,11 +5,11 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2017_1C\PrograAvanzada\tpComplejidad\Analisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mica\workspace\TallerProgra\fork_mramirez\tpComplejidad\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Polinomio" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Recursiva</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Usando matriz</t>
+  </si>
+  <si>
+    <t>Mejorada</t>
   </si>
 </sst>
 </file>
@@ -193,7 +196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -211,13 +214,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,19 +454,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
                 <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
@@ -476,85 +475,85 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>13</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>14</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>14</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>17</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>18</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>20</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>22</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>23</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>25</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>26</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>27</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>29</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -710,16 +709,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2</c:v>
@@ -743,13 +742,13 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>15</c:v>
@@ -758,28 +757,28 @@
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>19</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>23</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>25</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>27</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>31</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>37</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>39</c:v>
@@ -788,28 +787,28 @@
                   <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>44</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>52</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>55</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>59</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>62</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>67</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>71</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -968,7 +967,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -977,16 +976,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1</c:v>
@@ -1001,10 +1000,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1</c:v>
@@ -1019,43 +1018,43 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="20">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="22">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="24">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="25">
-                  <c:v>3</c:v>
-                </c:pt>
                 <c:pt idx="26">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>4</c:v>
@@ -1064,7 +1063,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1250,43 +1249,43 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>0</c:v>
@@ -1481,22 +1480,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1</c:v>
@@ -1511,13 +1510,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1</c:v>
@@ -1529,13 +1528,13 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>2</c:v>
@@ -1556,10 +1555,10 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="27">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="28">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>2</c:v>
@@ -1568,7 +1567,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>3</c:v>
@@ -1733,91 +1732,91 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>0</c:v>
@@ -1838,6 +1837,263 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-9CC4-4265-AA32-41AE1FDEF9E2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Polinomio!$H$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mejorada</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Polinomio!$A$4:$A$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2800</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3200</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3400</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3600</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3800</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4200</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4400</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4600</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4800</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5200</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5400</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5600</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5800</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6200</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6400</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6600</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>6800</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Polinomio!$H$4:$H$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0F9C-4725-80FA-9C9B73774066}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4035,19 +4291,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G51"/>
+  <dimension ref="A2:H51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>3</v>
       </c>
@@ -4059,8 +4316,9 @@
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="11"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -4080,16 +4338,19 @@
       <c r="G3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>400</v>
       </c>
       <c r="B4" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="3">
         <v>1</v>
@@ -4103,20 +4364,23 @@
       <c r="G4" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>600</v>
       </c>
       <c r="B5" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="3">
-        <v>0</v>
-      </c>
       <c r="E5" s="3">
         <v>0</v>
       </c>
@@ -4124,18 +4388,21 @@
         <v>0</v>
       </c>
       <c r="G5" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>800</v>
       </c>
       <c r="B6" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="3">
         <v>0</v>
@@ -4144,21 +4411,24 @@
         <v>0</v>
       </c>
       <c r="F6" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1000</v>
       </c>
       <c r="B7" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="3">
         <v>1</v>
@@ -4172,31 +4442,37 @@
       <c r="G7" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>1200</v>
       </c>
       <c r="B8" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" s="5">
         <v>2</v>
       </c>
       <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
         <v>1</v>
       </c>
-      <c r="E8" s="3">
-        <v>0</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0</v>
-      </c>
       <c r="G8" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>1400</v>
       </c>
@@ -4207,7 +4483,7 @@
         <v>3</v>
       </c>
       <c r="D9" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="3">
         <v>0</v>
@@ -4218,8 +4494,11 @@
       <c r="G9" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>1600</v>
       </c>
@@ -4236,36 +4515,42 @@
         <v>0</v>
       </c>
       <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3">
         <v>1</v>
       </c>
-      <c r="G10" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>1800</v>
       </c>
       <c r="B11" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11" s="5">
         <v>4</v>
       </c>
       <c r="D11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="3">
         <v>0</v>
       </c>
       <c r="F11" s="3">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3">
         <v>1</v>
       </c>
-      <c r="G11" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>2000</v>
       </c>
@@ -4287,13 +4572,16 @@
       <c r="G12" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>2200</v>
       </c>
       <c r="B13" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C13" s="5">
         <v>7</v>
@@ -4310,13 +4598,16 @@
       <c r="G13" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>2400</v>
       </c>
       <c r="B14" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C14" s="5">
         <v>8</v>
@@ -4325,7 +4616,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" s="3">
         <v>1</v>
@@ -4333,8 +4624,11 @@
       <c r="G14" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>2600</v>
       </c>
@@ -4342,7 +4636,7 @@
         <v>4</v>
       </c>
       <c r="C15" s="5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D15" s="3">
         <v>1</v>
@@ -4354,33 +4648,39 @@
         <v>1</v>
       </c>
       <c r="G15" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>2800</v>
       </c>
       <c r="B16" s="6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C16" s="5">
         <v>11</v>
       </c>
       <c r="D16" s="3">
+        <v>1</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
         <v>2</v>
       </c>
-      <c r="E16" s="3">
-        <v>0</v>
-      </c>
-      <c r="F16" s="3">
-        <v>1</v>
-      </c>
       <c r="G16" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>3000</v>
       </c>
@@ -4388,10 +4688,10 @@
         <v>6</v>
       </c>
       <c r="C17" s="5">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D17" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17" s="3">
         <v>0</v>
@@ -4400,15 +4700,18 @@
         <v>1</v>
       </c>
       <c r="G17" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>3200</v>
       </c>
       <c r="B18" s="6">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C18" s="5">
         <v>15</v>
@@ -4420,18 +4723,21 @@
         <v>0</v>
       </c>
       <c r="F18" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G18" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>3400</v>
       </c>
       <c r="B19" s="6">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C19" s="5">
         <v>16</v>
@@ -4448,16 +4754,19 @@
       <c r="G19" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>3600</v>
       </c>
       <c r="B20" s="6">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C20" s="5">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20" s="3">
         <v>2</v>
@@ -4469,15 +4778,18 @@
         <v>2</v>
       </c>
       <c r="G20" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>3800</v>
       </c>
       <c r="B21" s="6">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C21" s="5">
         <v>20</v>
@@ -4494,39 +4806,45 @@
       <c r="G21" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>4000</v>
       </c>
       <c r="B22" s="6">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C22" s="5">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D22" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22" s="3">
         <v>0</v>
       </c>
       <c r="F22" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G22" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="H22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>4200</v>
       </c>
       <c r="B23" s="6">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C23" s="5">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D23" s="3">
         <v>2</v>
@@ -4535,47 +4853,53 @@
         <v>0</v>
       </c>
       <c r="F23" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G23" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>4400</v>
       </c>
       <c r="B24" s="7">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C24" s="3">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D24" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E24" s="3">
         <v>0</v>
       </c>
       <c r="F24" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G24" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>4600</v>
       </c>
       <c r="B25" s="7">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C25" s="3">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D25" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E25" s="3">
         <v>0</v>
@@ -4586,22 +4910,25 @@
       <c r="G25" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>4800</v>
       </c>
       <c r="B26" s="7">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C26" s="3">
         <v>33</v>
       </c>
       <c r="D26" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E26" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="3">
         <v>2</v>
@@ -4609,16 +4936,19 @@
       <c r="G26" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>5000</v>
       </c>
       <c r="B27" s="7">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C27" s="3">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D27" s="3">
         <v>3</v>
@@ -4632,19 +4962,22 @@
       <c r="G27" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>5200</v>
       </c>
       <c r="B28" s="7">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C28" s="3">
         <v>39</v>
       </c>
       <c r="D28" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E28" s="3">
         <v>0</v>
@@ -4653,21 +4986,24 @@
         <v>2</v>
       </c>
       <c r="G28" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="H28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>5400</v>
       </c>
       <c r="B29" s="7">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C29" s="3">
         <v>42</v>
       </c>
       <c r="D29" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E29" s="3">
         <v>0</v>
@@ -4678,19 +5014,22 @@
       <c r="G29" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>5600</v>
       </c>
       <c r="B30" s="7">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C30" s="3">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D30" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E30" s="3">
         <v>0</v>
@@ -4701,16 +5040,19 @@
       <c r="G30" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>5800</v>
       </c>
       <c r="B31" s="7">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C31" s="3">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D31" s="3">
         <v>3</v>
@@ -4719,44 +5061,50 @@
         <v>0</v>
       </c>
       <c r="F31" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G31" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>6000</v>
       </c>
       <c r="B32" s="7">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C32" s="3">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D32" s="3">
+        <v>3</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0</v>
+      </c>
+      <c r="F32" s="3">
         <v>2</v>
       </c>
-      <c r="E32" s="3">
-        <v>0</v>
-      </c>
-      <c r="F32" s="3">
-        <v>3</v>
-      </c>
       <c r="G32" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>6200</v>
       </c>
       <c r="B33" s="7">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C33" s="3">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D33" s="3">
         <v>3</v>
@@ -4768,21 +5116,24 @@
         <v>2</v>
       </c>
       <c r="G33" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="H33" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>6400</v>
       </c>
       <c r="B34" s="7">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C34" s="3">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D34" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E34" s="3">
         <v>0</v>
@@ -4793,16 +5144,19 @@
       <c r="G34" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>6600</v>
       </c>
       <c r="B35" s="7">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C35" s="3">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D35" s="3">
         <v>4</v>
@@ -4811,21 +5165,24 @@
         <v>0</v>
       </c>
       <c r="F35" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G35" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>6800</v>
       </c>
       <c r="B36" s="7">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C36" s="3">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="D36" s="3">
         <v>3</v>
@@ -4839,19 +5196,22 @@
       <c r="G36" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>7000</v>
       </c>
       <c r="B37" s="8">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C37" s="4">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D37" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E37" s="4">
         <v>0</v>
@@ -4862,8 +5222,11 @@
       <c r="G37" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="10"/>
       <c r="B38" s="10"/>
       <c r="C38" s="10"/>
@@ -4872,7 +5235,7 @@
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
@@ -4881,7 +5244,7 @@
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
@@ -4890,7 +5253,7 @@
       <c r="F40" s="10"/>
       <c r="G40" s="10"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="B41" s="10"/>
       <c r="C41" s="10"/>
@@ -4899,7 +5262,7 @@
       <c r="F41" s="10"/>
       <c r="G41" s="10"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
@@ -4908,7 +5271,7 @@
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
@@ -4917,7 +5280,7 @@
       <c r="F43" s="10"/>
       <c r="G43" s="10"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
@@ -4926,7 +5289,7 @@
       <c r="F44" s="10"/>
       <c r="G44" s="10"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
@@ -4935,7 +5298,7 @@
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
@@ -4944,7 +5307,7 @@
       <c r="F46" s="10"/>
       <c r="G46" s="10"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
@@ -4953,7 +5316,7 @@
       <c r="F47" s="10"/>
       <c r="G47" s="10"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
@@ -4991,8 +5354,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B2:G2"/>
     <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5004,8 +5367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5022,22 +5385,22 @@
       <c r="B1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>